<commit_message>
Reverted to old method of calculating reversibilities for some cases
</commit_message>
<xml_diff>
--- a/input_test/HMP1489_r1_t0.xlsx
+++ b/input_test/HMP1489_r1_t0.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="12"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="1" state="visible" r:id="rId2"/>
@@ -516,8 +516,8 @@
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="1" sqref="C4 B8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -570,7 +570,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>10000</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -653,7 +653,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -748,7 +748,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -929,7 +929,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1207,15 +1207,15 @@
   </sheetPr>
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="40.919028340081"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.1538461538462"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="41.5627530364373"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="51.9514170040486"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1479,7 +1479,7 @@
   <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2122,7 +2122,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2455,7 +2455,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2636,7 +2636,7 @@
   <dimension ref="A2:A12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2718,7 +2718,7 @@
   <dimension ref="A2:A19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2835,7 +2835,7 @@
   <dimension ref="A2:A19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2952,7 +2952,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="C4 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3100,7 +3100,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="C4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>